<commit_message>
updated excel file with intents
</commit_message>
<xml_diff>
--- a/backend/intents.xlsx
+++ b/backend/intents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Minh-Kha\Projects\versus-virus-chatbot\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05529820-2AC0-4E93-96ED-B4FE0ABE82E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC848E53-CF4B-42C3-A180-28BEA8D4D7D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E51EFE97-ECD2-4DE9-A916-037E6E1F97F0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>intent</t>
   </si>
@@ -47,16 +47,74 @@
     <t>leistung</t>
   </si>
   <si>
-    <t>antrag</t>
-  </si>
-  <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>xyz</t>
-  </si>
-  <si>
-    <t>sdf</t>
+    <t>allgemein</t>
+  </si>
+  <si>
+    <t>anmeldung</t>
+  </si>
+  <si>
+    <t>auszahlung</t>
+  </si>
+  <si>
+    <t>einfuehrung</t>
+  </si>
+  <si>
+    <t>verfuegung</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Einen Anspruch kann der Arbeitgeber für jene Arbeitnehmenden geltend machen, welche die obligatorische Schule abgeschlossen und das AHV-Rentenalter noch nicht erreicht haben. Aufgrund der ausserordentlichen Lage haben ausnahmsweise vorübergehend auch weitere Personengruppen Anspruch auf Kurzarbeitsentschädigung: \n
+- Personen in einem Arbeitsverhältnis auf bestimmte Dauer (**befristete** Arbeitsverhältnisse) \n
+- Personen in einem Lehrverhältnis (**Lernende** und Lehrmeister) \n
+- Personen im Dienste einer Organisation für **Temporärarbeit** \n
+- Personen in **arbeitgeberähnlicher** Stellung, die nach dem Bundesgesetz über die Alters- und Hinterbliebenenversicherung (AHVG) als unselbstständig Erwerbende Lohn erzielen.</t>
+  </si>
+  <si>
+    <t>Wenn Sie fehlende Angaben nachreichen müssen, erhalten Sie eine entsprechende Aufforderung telefonisch oder per E-Mail.\n
+Die Verfügung teilt Ihnen mit:\n
+\n
+- «Gegen die Auszahlung Kurzarbeitsentschädigung erheben wir keinen Einspruch.» Das heisst, die Voranmeldung für Kurzarbeit wurde bewilligt. Die Bewilligungsdauer beträgt aufgrund der aktuellen Situation neu 6 Monate. \n
+- «Gegen die Auszahlung Kurzarbeitsentschädigung erheben wir teilweise Einspruch.» Das heisst, die Voranmeldung für Kurzarbeit wurde teilweise bewilligt. Dies bezieht sich in den meisten Fällen auf die Bewilligungsdauer oder andere Gründe, die in der Verfügung beschrieben werden. \n
+- «Gegen die Auszahlung Kurzarbeitsentschädigung erheben wir Einspruch.» Das heisst, die Voranmeldung für Kurzarbeit wurde nicht bewilligt. \n
+\n
+Die Verfügung wird auch der Arbeitslosenkasse mitgeteilt, die Sie auf dem Formular «Voranmeldung von Kurzarbeit» angegeben haben.</t>
+  </si>
+  <si>
+    <t>1. Holen Sie zuerst das Einverständnis aller von Kurzarbeit betroffenen Mitarbeitenden mit der Einführung von Kurzarbeit ein. Sie müssen dieses Einverständnis im Formular schriftlich bestätigen. \n
+2. Füllen Sie das Formular «Voranmeldung von Kurzarbeit» aus und unterschreiben Sie es. Im Formular müssen Sie bestimmen, von welcher Arbeitslosenkasse Sie die Kurzarbeitsentschädigung beziehen wollen. \n
+3. Legen Sie das Organigramm des Gesamtbetriebes bei. Geben Sie bei Betriebsabteilungen auch die Anzahl der Mitarbeitenden pro Organisationseinheit an.
+4. Reichen Sie die Unterlagen per E-Mail (voranmeldung.kurzarbeit@vd.zh.ch) oder postalisch unter folgender Adresse ein: \n
+\n
+Amt für Wirtschaft und Arbeit\n
+Arbeitslosenversicherung\n
+Kurzarbeit\n
+Stampfenbachstrasse 32\n
+8090 Zürich</t>
+  </si>
+  <si>
+    <t>Ich habe Ihre Frage leider nicht verstanden.</t>
+  </si>
+  <si>
+    <t>- Ab Einführung von Kurzarbeit besteht Anspruch auf Kurzarbeitsentschädigung. Der Poststempel der Voranmeldung für Kurzarbeit bzw. das Datum ihres Eingangs per E-Mail bilden den Termin, mit dem die Bewilligungsdauer beginnt.\n
+- Ab Einführung von Kurzarbeit müssen Sie Arbeitszeitlisten oder Stundenrapports (Excel-Tabelle) führen bzw. einen entsprechenden Nachweis des Ausfalls. Dies dient der Arbeitslosenkasse zur Kontrolle der Soll- und Ausfallstunden. \n
+- Die Abrechnung der Arbeitslosenentschädigung erfolgt ab Beginn der Kurzarbeit bis zum Monatsende. Die Abrechnungsperiode beträgt 1 Monat (Kalendermonat). Somit wird jeder Monat separat abgerechnet. Die Abrechnung muss innert 3 Monaten nach Beendigung der Abrechnungsperiode eingereicht werden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Höhe der Kurzarbeitsentschädigung wird monatlich auf Basis des  Formulars «Antrag und Abrechnung von Kurzarbeitsentschädigung (COVID-19) (d/f/i)» bestimmt. Bitte befolgen Sie die folgenden Anweisungen bei dem Ausfüllen des Formulars, um eine effiziente Bearbeitung und schnellstmögliche Auszahlung zu gewährleisten. \n
+\n
+- Füllen Sie das Formular «Antrag und Abrechnung von Kurzarbeitsentschädigung» mit dem **Computer** aus und unterschreiben Sie es. Vergessen Sie nicht die **BUR-Nr.** und die **IBAN-Nr.** (Sie finden die BUR-Nr. auf der Verfügung der Arbeitslosenversicherung).\n
+- Nachweis des Totals der Soll-Stunden (Arbeitszeitliste oder Stundenrapport) für die anspruchsberechtigte Abrechnungsperiode: heben Sie das Total **deutlich** hervor. \n
+- Nachweis des Totals der AHV-pflichtigen Lohnsumme (Lohnjournal) für die anspruchsberechtigte Abrechnungsperiode: heben Sie das Total **deutlich** hervor. \n
+- Reichen Sie die Unterlagen per Post an die von Ihnen im Formular **«Voranmeldung von Kurzarbeit»** gewählte Arbeitslosenkasse ein.  </t>
+  </si>
+  <si>
+    <t>- Die Auszahlung erfolgt an die Kontoverbindung, die Sie im Formular «Antrag und Abrechnung von Kurzarbeitsentschädigung» angegeben haben. \n
+- Aufgrund der sehr hohen Zahl von Anträgen, die wir täglich erhalten, wird die Bearbeitung einige Zeit in Anspruch nehmen. Es kann zu Verzögerungen bei der Auszahlung kommen.</t>
+  </si>
+  <si>
+    <t>Betriebe und vorübergehend auch weitere Personengruppen können Kurzarbeit anmelden, wenn ihre Arbeitsausfälle im Zusammenhang mit dem Coronavirus stehen. Dank der Kurzarbeitsentschädigung können Teillöhne weiterbezahlt, Arbeitsplätze erhalten und Arbeitslosigkeit vermieden werden.</t>
   </si>
 </sst>
 </file>
@@ -92,8 +150,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,44 +473,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82CBFD14-179D-4616-A167-13E697E3E5E0}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="167.21875" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>